<commit_message>
Modified CO components CT2 marks for CO2 and CO3, CT3 marks for CO4 and CO5
</commit_message>
<xml_diff>
--- a/output/result.xlsx
+++ b/output/result.xlsx
@@ -590,7 +590,11 @@
       <c r="AC1" s="2" t="n"/>
       <c r="AD1" s="2" t="n"/>
       <c r="AE1" s="2" t="n"/>
-      <c r="AF1" s="2" t="n"/>
+      <c r="AF1" s="1" t="inlineStr">
+        <is>
+          <t>FT-II , FT-IV</t>
+        </is>
+      </c>
       <c r="AG1" s="2" t="n"/>
       <c r="AH1" s="2" t="n"/>
       <c r="AI1" s="2" t="n"/>
@@ -614,7 +618,11 @@
       <c r="AW1" s="2" t="n"/>
       <c r="AX1" s="2" t="n"/>
       <c r="AY1" s="2" t="n"/>
-      <c r="AZ1" s="2" t="n"/>
+      <c r="AZ1" s="1" t="inlineStr">
+        <is>
+          <t>FT-III, REPORT</t>
+        </is>
+      </c>
       <c r="BA1" s="2" t="n"/>
       <c r="BB1" s="2" t="n"/>
       <c r="BC1" s="2" t="n"/>
@@ -668,7 +676,11 @@
       <c r="AC2" s="2" t="n"/>
       <c r="AD2" s="2" t="n"/>
       <c r="AE2" s="2" t="n"/>
-      <c r="AF2" s="2" t="n"/>
+      <c r="AF2" s="3" t="inlineStr">
+        <is>
+          <t>CO3</t>
+        </is>
+      </c>
       <c r="AG2" s="2" t="n"/>
       <c r="AH2" s="2" t="n"/>
       <c r="AI2" s="2" t="n"/>
@@ -680,7 +692,7 @@
       <c r="AO2" s="2" t="n"/>
       <c r="AP2" s="3" t="inlineStr">
         <is>
-          <t>CO3</t>
+          <t>CO4</t>
         </is>
       </c>
       <c r="AQ2" s="2" t="n"/>
@@ -692,7 +704,11 @@
       <c r="AW2" s="2" t="n"/>
       <c r="AX2" s="2" t="n"/>
       <c r="AY2" s="2" t="n"/>
-      <c r="AZ2" s="2" t="n"/>
+      <c r="AZ2" s="3" t="inlineStr">
+        <is>
+          <t>CO5</t>
+        </is>
+      </c>
       <c r="BA2" s="2" t="n"/>
       <c r="BB2" s="2" t="n"/>
       <c r="BC2" s="2" t="n"/>
@@ -708,9 +724,7 @@
       <c r="C3" s="2" t="n"/>
       <c r="D3" s="4" t="inlineStr">
         <is>
-          <t>THEORY 
- (for either/or Q, 
- award marks for the attempted students only)</t>
+          <t>THEORY (for either/or Q, award marks for the attempted students only)</t>
         </is>
       </c>
       <c r="E3" s="2" t="n"/>
@@ -733,9 +747,7 @@
       <c r="V3" s="2" t="n"/>
       <c r="W3" s="4" t="inlineStr">
         <is>
-          <t>THEORY 
- (for either/or Q, 
- award marks for the attempted students only)</t>
+          <t>THEORY (for either/or Q, award marks for the attempted students only)</t>
         </is>
       </c>
       <c r="X3" s="2" t="n"/>
@@ -746,7 +758,11 @@
       <c r="AC3" s="2" t="n"/>
       <c r="AD3" s="2" t="n"/>
       <c r="AE3" s="2" t="n"/>
-      <c r="AF3" s="2" t="n"/>
+      <c r="AF3" s="4" t="inlineStr">
+        <is>
+          <t>THEORY (for either/or Q, award marks for the attempted students only)</t>
+        </is>
+      </c>
       <c r="AG3" s="2" t="n"/>
       <c r="AH3" s="2" t="n"/>
       <c r="AI3" s="2" t="n"/>
@@ -758,9 +774,7 @@
       <c r="AO3" s="2" t="n"/>
       <c r="AP3" s="4" t="inlineStr">
         <is>
-          <t>THEORY 
- (for either/or Q, 
- award marks for the attempted students only)</t>
+          <t>THEORY (for either/or Q, award marks for the attempted students only)</t>
         </is>
       </c>
       <c r="AQ3" s="2" t="n"/>
@@ -772,7 +786,11 @@
       <c r="AW3" s="2" t="n"/>
       <c r="AX3" s="2" t="n"/>
       <c r="AY3" s="2" t="n"/>
-      <c r="AZ3" s="2" t="n"/>
+      <c r="AZ3" s="4" t="inlineStr">
+        <is>
+          <t>THEORY (for either/or Q, award marks for the attempted students only)</t>
+        </is>
+      </c>
       <c r="BA3" s="2" t="n"/>
       <c r="BB3" s="2" t="n"/>
       <c r="BC3" s="2" t="n"/>
@@ -866,13 +884,13 @@
         <v>1</v>
       </c>
       <c r="AC4" s="7" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="AD4" s="7" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="AE4" s="7" t="n">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="AF4" s="7" t="n">
         <v>1</v>
@@ -881,13 +899,13 @@
         <v>1</v>
       </c>
       <c r="AH4" s="7" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="AI4" s="7" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="AJ4" s="7" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="AK4" s="7" t="n">
         <v>8</v>
@@ -899,7 +917,7 @@
         <v>8</v>
       </c>
       <c r="AN4" s="7" t="n">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="AO4" s="7" t="n">
         <v>15</v>
@@ -923,31 +941,31 @@
         <v>1</v>
       </c>
       <c r="AV4" s="7" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="AW4" s="7" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="AX4" s="7" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="AY4" s="7" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="AZ4" s="7" t="n">
         <v>1</v>
       </c>
       <c r="BA4" s="7" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="BB4" s="7" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="BC4" s="7" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="BD4" s="7" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="BE4" s="7" t="n">
         <v>8</v>
@@ -1002,7 +1020,11 @@
       <c r="AC5" s="2" t="n"/>
       <c r="AD5" s="2" t="n"/>
       <c r="AE5" s="2" t="n"/>
-      <c r="AF5" s="2" t="n"/>
+      <c r="AF5" s="8" t="inlineStr">
+        <is>
+          <t>Question numbers mapping</t>
+        </is>
+      </c>
       <c r="AG5" s="2" t="n"/>
       <c r="AH5" s="2" t="n"/>
       <c r="AI5" s="2" t="n"/>
@@ -1026,7 +1048,11 @@
       <c r="AW5" s="2" t="n"/>
       <c r="AX5" s="2" t="n"/>
       <c r="AY5" s="2" t="n"/>
-      <c r="AZ5" s="2" t="n"/>
+      <c r="AZ5" s="8" t="inlineStr">
+        <is>
+          <t>Question numbers mapping</t>
+        </is>
+      </c>
       <c r="BA5" s="2" t="n"/>
       <c r="BB5" s="2" t="n"/>
       <c r="BC5" s="2" t="n"/>
@@ -1179,142 +1205,142 @@
       </c>
       <c r="AC6" s="4" t="inlineStr">
         <is>
+          <t>Q12.A</t>
+        </is>
+      </c>
+      <c r="AD6" s="4" t="inlineStr">
+        <is>
+          <t>Q12.B</t>
+        </is>
+      </c>
+      <c r="AE6" s="4" t="inlineStr">
+        <is>
+          <t>Q15</t>
+        </is>
+      </c>
+      <c r="AF6" s="4" t="inlineStr">
+        <is>
           <t>Q7</t>
         </is>
       </c>
-      <c r="AD6" s="4" t="inlineStr">
+      <c r="AG6" s="4" t="inlineStr">
         <is>
           <t>Q8</t>
         </is>
       </c>
-      <c r="AE6" s="4" t="inlineStr">
+      <c r="AH6" s="4" t="inlineStr">
         <is>
           <t>Q9</t>
         </is>
       </c>
-      <c r="AF6" s="4" t="inlineStr">
+      <c r="AI6" s="4" t="inlineStr">
         <is>
           <t>Q10</t>
         </is>
       </c>
-      <c r="AG6" s="4" t="inlineStr">
+      <c r="AJ6" s="4" t="inlineStr">
         <is>
           <t>Q11</t>
         </is>
       </c>
-      <c r="AH6" s="4" t="inlineStr">
+      <c r="AK6" s="4" t="inlineStr">
+        <is>
+          <t>Q13.A</t>
+        </is>
+      </c>
+      <c r="AL6" s="4" t="inlineStr">
+        <is>
+          <t>Q13.B</t>
+        </is>
+      </c>
+      <c r="AM6" s="4" t="inlineStr">
+        <is>
+          <t>Q14.A</t>
+        </is>
+      </c>
+      <c r="AN6" s="4" t="inlineStr">
+        <is>
+          <t>Q14.B</t>
+        </is>
+      </c>
+      <c r="AO6" s="4" t="inlineStr">
+        <is>
+          <t>Q16</t>
+        </is>
+      </c>
+      <c r="AP6" s="4" t="inlineStr">
+        <is>
+          <t>Q1</t>
+        </is>
+      </c>
+      <c r="AQ6" s="4" t="inlineStr">
+        <is>
+          <t>Q2</t>
+        </is>
+      </c>
+      <c r="AR6" s="4" t="inlineStr">
+        <is>
+          <t>Q3</t>
+        </is>
+      </c>
+      <c r="AS6" s="4" t="inlineStr">
+        <is>
+          <t>Q4</t>
+        </is>
+      </c>
+      <c r="AT6" s="4" t="inlineStr">
+        <is>
+          <t>Q5</t>
+        </is>
+      </c>
+      <c r="AU6" s="4" t="inlineStr">
+        <is>
+          <t>Q6</t>
+        </is>
+      </c>
+      <c r="AV6" s="4" t="inlineStr">
         <is>
           <t>Q12.A</t>
         </is>
       </c>
-      <c r="AI6" s="4" t="inlineStr">
+      <c r="AW6" s="4" t="inlineStr">
         <is>
           <t>Q12.B</t>
         </is>
       </c>
-      <c r="AJ6" s="4" t="inlineStr">
+      <c r="AX6" s="4" t="inlineStr">
         <is>
           <t>Q13.A</t>
         </is>
       </c>
-      <c r="AK6" s="4" t="inlineStr">
+      <c r="AY6" s="4" t="inlineStr">
         <is>
           <t>Q13.B</t>
         </is>
       </c>
-      <c r="AL6" s="4" t="inlineStr">
-        <is>
-          <t>Q14.A</t>
-        </is>
-      </c>
-      <c r="AM6" s="4" t="inlineStr">
-        <is>
-          <t>Q14.B</t>
-        </is>
-      </c>
-      <c r="AN6" s="4" t="inlineStr">
-        <is>
-          <t>Q15</t>
-        </is>
-      </c>
-      <c r="AO6" s="4" t="inlineStr">
-        <is>
-          <t>Q16</t>
-        </is>
-      </c>
-      <c r="AP6" s="4" t="inlineStr">
-        <is>
-          <t>Q1</t>
-        </is>
-      </c>
-      <c r="AQ6" s="4" t="inlineStr">
-        <is>
-          <t>Q2</t>
-        </is>
-      </c>
-      <c r="AR6" s="4" t="inlineStr">
-        <is>
-          <t>Q3</t>
-        </is>
-      </c>
-      <c r="AS6" s="4" t="inlineStr">
-        <is>
-          <t>Q4</t>
-        </is>
-      </c>
-      <c r="AT6" s="4" t="inlineStr">
-        <is>
-          <t>Q5</t>
-        </is>
-      </c>
-      <c r="AU6" s="4" t="inlineStr">
-        <is>
-          <t>Q6</t>
-        </is>
-      </c>
-      <c r="AV6" s="4" t="inlineStr">
+      <c r="AZ6" s="4" t="inlineStr">
         <is>
           <t>Q7</t>
         </is>
       </c>
-      <c r="AW6" s="4" t="inlineStr">
+      <c r="BA6" s="4" t="inlineStr">
         <is>
           <t>Q8</t>
         </is>
       </c>
-      <c r="AX6" s="4" t="inlineStr">
+      <c r="BB6" s="4" t="inlineStr">
         <is>
           <t>Q9</t>
         </is>
       </c>
-      <c r="AY6" s="4" t="inlineStr">
+      <c r="BC6" s="4" t="inlineStr">
         <is>
           <t>Q10</t>
         </is>
       </c>
-      <c r="AZ6" s="4" t="inlineStr">
+      <c r="BD6" s="4" t="inlineStr">
         <is>
           <t>Q11</t>
-        </is>
-      </c>
-      <c r="BA6" s="4" t="inlineStr">
-        <is>
-          <t>Q12.A</t>
-        </is>
-      </c>
-      <c r="BB6" s="4" t="inlineStr">
-        <is>
-          <t>Q12.B</t>
-        </is>
-      </c>
-      <c r="BC6" s="4" t="inlineStr">
-        <is>
-          <t>Q13.A</t>
-        </is>
-      </c>
-      <c r="BD6" s="4" t="inlineStr">
-        <is>
-          <t>Q13.B</t>
         </is>
       </c>
       <c r="BE6" s="4" t="inlineStr">
@@ -1339,22 +1365,30 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="23">
+    <mergeCell ref="AF5:AO5"/>
+    <mergeCell ref="AF2:AO2"/>
+    <mergeCell ref="AP2:AY2"/>
+    <mergeCell ref="W1:AE1"/>
+    <mergeCell ref="AZ5:BH5"/>
+    <mergeCell ref="D3:V3"/>
+    <mergeCell ref="W3:AE3"/>
+    <mergeCell ref="AF1:AO1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="D5:V5"/>
+    <mergeCell ref="AF3:AO3"/>
+    <mergeCell ref="AP3:AY3"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="W2:AE2"/>
     <mergeCell ref="D1:V1"/>
-    <mergeCell ref="D5:V5"/>
-    <mergeCell ref="W1:AO1"/>
+    <mergeCell ref="AZ3:BH3"/>
+    <mergeCell ref="AZ2:BH2"/>
+    <mergeCell ref="AP5:AY5"/>
+    <mergeCell ref="D2:V2"/>
+    <mergeCell ref="AP1:AY1"/>
     <mergeCell ref="A1:C1"/>
-    <mergeCell ref="AP2:BH2"/>
-    <mergeCell ref="AP1:BH1"/>
-    <mergeCell ref="W3:AO3"/>
-    <mergeCell ref="AP5:BH5"/>
-    <mergeCell ref="D3:V3"/>
-    <mergeCell ref="W5:AO5"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="AP3:BH3"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="W2:AO2"/>
-    <mergeCell ref="D2:V2"/>
+    <mergeCell ref="AZ1:BH1"/>
+    <mergeCell ref="W5:AE5"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Modified row 1 FT components to merge CO components
</commit_message>
<xml_diff>
--- a/output/result.xlsx
+++ b/output/result.xlsx
@@ -590,11 +590,7 @@
       <c r="AC1" s="2" t="n"/>
       <c r="AD1" s="2" t="n"/>
       <c r="AE1" s="2" t="n"/>
-      <c r="AF1" s="1" t="inlineStr">
-        <is>
-          <t>FT-II , FT-IV</t>
-        </is>
-      </c>
+      <c r="AF1" s="2" t="n"/>
       <c r="AG1" s="2" t="n"/>
       <c r="AH1" s="2" t="n"/>
       <c r="AI1" s="2" t="n"/>
@@ -618,11 +614,7 @@
       <c r="AW1" s="2" t="n"/>
       <c r="AX1" s="2" t="n"/>
       <c r="AY1" s="2" t="n"/>
-      <c r="AZ1" s="1" t="inlineStr">
-        <is>
-          <t>FT-III, REPORT</t>
-        </is>
-      </c>
+      <c r="AZ1" s="2" t="n"/>
       <c r="BA1" s="2" t="n"/>
       <c r="BB1" s="2" t="n"/>
       <c r="BC1" s="2" t="n"/>
@@ -1365,15 +1357,13 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="23">
+  <mergeCells count="21">
     <mergeCell ref="AF5:AO5"/>
     <mergeCell ref="AF2:AO2"/>
     <mergeCell ref="AP2:AY2"/>
-    <mergeCell ref="W1:AE1"/>
     <mergeCell ref="AZ5:BH5"/>
     <mergeCell ref="D3:V3"/>
     <mergeCell ref="W3:AE3"/>
-    <mergeCell ref="AF1:AO1"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="D5:V5"/>
     <mergeCell ref="AF3:AO3"/>
@@ -1385,9 +1375,9 @@
     <mergeCell ref="AZ2:BH2"/>
     <mergeCell ref="AP5:AY5"/>
     <mergeCell ref="D2:V2"/>
-    <mergeCell ref="AP1:AY1"/>
+    <mergeCell ref="W1:AO1"/>
     <mergeCell ref="A1:C1"/>
-    <mergeCell ref="AZ1:BH1"/>
+    <mergeCell ref="AP1:BH1"/>
     <mergeCell ref="W5:AE5"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Modified logic for CO Attainment formulas and Unit tested
</commit_message>
<xml_diff>
--- a/output/result.xlsx
+++ b/output/result.xlsx
@@ -488,7 +488,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BB76"/>
+  <dimension ref="A1:BE76"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -497,59 +497,62 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="6" customWidth="1" min="1" max="1"/>
-    <col width="20" customWidth="1" min="2" max="2"/>
-    <col width="40" customWidth="1" min="3" max="3"/>
-    <col width="6" customWidth="1" min="4" max="4"/>
-    <col width="6" customWidth="1" min="5" max="5"/>
-    <col width="6" customWidth="1" min="6" max="6"/>
-    <col width="6" customWidth="1" min="7" max="7"/>
-    <col width="6" customWidth="1" min="8" max="8"/>
-    <col width="6" customWidth="1" min="9" max="9"/>
-    <col width="6" customWidth="1" min="10" max="10"/>
-    <col width="6" customWidth="1" min="11" max="11"/>
-    <col width="6" customWidth="1" min="12" max="12"/>
-    <col width="6" customWidth="1" min="13" max="13"/>
-    <col width="6" customWidth="1" min="14" max="14"/>
-    <col width="6" customWidth="1" min="15" max="15"/>
-    <col width="6" customWidth="1" min="16" max="16"/>
-    <col width="6" customWidth="1" min="17" max="17"/>
-    <col width="6" customWidth="1" min="18" max="18"/>
-    <col width="6" customWidth="1" min="19" max="19"/>
-    <col width="6" customWidth="1" min="20" max="20"/>
-    <col width="6" customWidth="1" min="21" max="21"/>
-    <col width="6" customWidth="1" min="22" max="22"/>
-    <col width="6" customWidth="1" min="23" max="23"/>
-    <col width="6" customWidth="1" min="24" max="24"/>
-    <col width="6" customWidth="1" min="25" max="25"/>
-    <col width="6" customWidth="1" min="26" max="26"/>
-    <col width="6" customWidth="1" min="27" max="27"/>
-    <col width="6" customWidth="1" min="28" max="28"/>
-    <col width="6" customWidth="1" min="29" max="29"/>
-    <col width="6" customWidth="1" min="30" max="30"/>
-    <col width="6" customWidth="1" min="31" max="31"/>
-    <col width="6" customWidth="1" min="32" max="32"/>
-    <col width="6" customWidth="1" min="33" max="33"/>
-    <col width="6" customWidth="1" min="34" max="34"/>
-    <col width="6" customWidth="1" min="35" max="35"/>
-    <col width="6" customWidth="1" min="36" max="36"/>
-    <col width="6" customWidth="1" min="37" max="37"/>
-    <col width="6" customWidth="1" min="38" max="38"/>
-    <col width="6" customWidth="1" min="39" max="39"/>
-    <col width="6" customWidth="1" min="40" max="40"/>
-    <col width="6" customWidth="1" min="41" max="41"/>
-    <col width="6" customWidth="1" min="42" max="42"/>
-    <col width="6" customWidth="1" min="43" max="43"/>
-    <col width="6" customWidth="1" min="44" max="44"/>
-    <col width="6" customWidth="1" min="45" max="45"/>
-    <col width="6" customWidth="1" min="46" max="46"/>
-    <col width="6" customWidth="1" min="47" max="47"/>
-    <col width="6" customWidth="1" min="48" max="48"/>
-    <col width="6" customWidth="1" min="49" max="49"/>
-    <col width="6" customWidth="1" min="50" max="50"/>
-    <col width="6" customWidth="1" min="51" max="51"/>
-    <col width="6" customWidth="1" min="52" max="52"/>
-    <col width="6" customWidth="1" min="53" max="53"/>
-    <col width="6" customWidth="1" min="54" max="54"/>
+    <col width="21" customWidth="1" min="2" max="2"/>
+    <col width="42" customWidth="1" min="3" max="3"/>
+    <col width="7" customWidth="1" min="4" max="4"/>
+    <col width="7" customWidth="1" min="5" max="5"/>
+    <col width="7" customWidth="1" min="6" max="6"/>
+    <col width="7" customWidth="1" min="7" max="7"/>
+    <col width="7" customWidth="1" min="8" max="8"/>
+    <col width="7" customWidth="1" min="9" max="9"/>
+    <col width="7" customWidth="1" min="10" max="10"/>
+    <col width="7" customWidth="1" min="11" max="11"/>
+    <col width="7" customWidth="1" min="12" max="12"/>
+    <col width="7" customWidth="1" min="13" max="13"/>
+    <col width="7" customWidth="1" min="14" max="14"/>
+    <col width="7" customWidth="1" min="15" max="15"/>
+    <col width="7" customWidth="1" min="16" max="16"/>
+    <col width="7" customWidth="1" min="17" max="17"/>
+    <col width="7" customWidth="1" min="18" max="18"/>
+    <col width="7" customWidth="1" min="19" max="19"/>
+    <col width="7" customWidth="1" min="20" max="20"/>
+    <col width="7" customWidth="1" min="21" max="21"/>
+    <col width="7" customWidth="1" min="22" max="22"/>
+    <col width="7" customWidth="1" min="23" max="23"/>
+    <col width="7" customWidth="1" min="24" max="24"/>
+    <col width="7" customWidth="1" min="25" max="25"/>
+    <col width="7" customWidth="1" min="26" max="26"/>
+    <col width="7" customWidth="1" min="27" max="27"/>
+    <col width="7" customWidth="1" min="28" max="28"/>
+    <col width="7" customWidth="1" min="29" max="29"/>
+    <col width="7" customWidth="1" min="30" max="30"/>
+    <col width="7" customWidth="1" min="31" max="31"/>
+    <col width="7" customWidth="1" min="32" max="32"/>
+    <col width="7" customWidth="1" min="33" max="33"/>
+    <col width="7" customWidth="1" min="34" max="34"/>
+    <col width="7" customWidth="1" min="35" max="35"/>
+    <col width="7" customWidth="1" min="36" max="36"/>
+    <col width="7" customWidth="1" min="37" max="37"/>
+    <col width="7" customWidth="1" min="38" max="38"/>
+    <col width="7" customWidth="1" min="39" max="39"/>
+    <col width="7" customWidth="1" min="40" max="40"/>
+    <col width="7" customWidth="1" min="41" max="41"/>
+    <col width="7" customWidth="1" min="42" max="42"/>
+    <col width="7" customWidth="1" min="43" max="43"/>
+    <col width="7" customWidth="1" min="44" max="44"/>
+    <col width="7" customWidth="1" min="45" max="45"/>
+    <col width="7" customWidth="1" min="46" max="46"/>
+    <col width="7" customWidth="1" min="47" max="47"/>
+    <col width="7" customWidth="1" min="48" max="48"/>
+    <col width="7" customWidth="1" min="49" max="49"/>
+    <col width="7" customWidth="1" min="50" max="50"/>
+    <col width="7" customWidth="1" min="51" max="51"/>
+    <col width="7" customWidth="1" min="52" max="52"/>
+    <col width="7" customWidth="1" min="53" max="53"/>
+    <col width="7" customWidth="1" min="54" max="54"/>
+    <col width="7" customWidth="1" min="55" max="55"/>
+    <col width="7" customWidth="1" min="56" max="56"/>
+    <col width="7" customWidth="1" min="57" max="57"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -623,6 +626,9 @@
       <c r="AZ1" s="1" t="n"/>
       <c r="BA1" s="1" t="n"/>
       <c r="BB1" s="1" t="n"/>
+      <c r="BC1" s="1" t="n"/>
+      <c r="BD1" s="1" t="n"/>
+      <c r="BE1" s="1" t="n"/>
     </row>
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
@@ -681,7 +687,7 @@
       <c r="AL2" s="3" t="n"/>
       <c r="AM2" s="3" t="inlineStr">
         <is>
-          <t>CO1</t>
+          <t>CO2</t>
         </is>
       </c>
       <c r="AN2" s="3" t="n"/>
@@ -690,7 +696,11 @@
       <c r="AQ2" s="3" t="n"/>
       <c r="AR2" s="3" t="n"/>
       <c r="AS2" s="3" t="n"/>
-      <c r="AT2" s="3" t="n"/>
+      <c r="AT2" s="3" t="inlineStr">
+        <is>
+          <t>CO3</t>
+        </is>
+      </c>
       <c r="AU2" s="3" t="n"/>
       <c r="AV2" s="3" t="n"/>
       <c r="AW2" s="3" t="n"/>
@@ -699,16 +709,19 @@
       <c r="AZ2" s="3" t="n"/>
       <c r="BA2" s="3" t="n"/>
       <c r="BB2" s="3" t="n"/>
+      <c r="BC2" s="3" t="n"/>
+      <c r="BD2" s="3" t="n"/>
+      <c r="BE2" s="3" t="n"/>
     </row>
     <row r="3">
-      <c r="A3" s="5" t="n"/>
+      <c r="A3" s="5" t="inlineStr">
+        <is>
+          <t>THEORY (for either/or Q, award marks for the attempted students only)</t>
+        </is>
+      </c>
       <c r="B3" s="5" t="n"/>
       <c r="C3" s="6" t="n"/>
-      <c r="D3" s="5" t="inlineStr">
-        <is>
-          <t>THEORY (for either/or Q, award marks for the attempted students only)</t>
-        </is>
-      </c>
+      <c r="D3" s="5" t="n"/>
       <c r="E3" s="5" t="n"/>
       <c r="F3" s="5" t="n"/>
       <c r="G3" s="5" t="n"/>
@@ -724,11 +737,7 @@
       <c r="Q3" s="5" t="n"/>
       <c r="R3" s="5" t="n"/>
       <c r="S3" s="5" t="n"/>
-      <c r="T3" s="5" t="inlineStr">
-        <is>
-          <t>THEORY (for either/or Q, award marks for the attempted students only)</t>
-        </is>
-      </c>
+      <c r="T3" s="5" t="n"/>
       <c r="U3" s="5" t="n"/>
       <c r="V3" s="5" t="n"/>
       <c r="W3" s="5" t="n"/>
@@ -747,11 +756,7 @@
       <c r="AJ3" s="5" t="n"/>
       <c r="AK3" s="5" t="n"/>
       <c r="AL3" s="5" t="n"/>
-      <c r="AM3" s="5" t="inlineStr">
-        <is>
-          <t>THEORY (for either/or Q, award marks for the attempted students only)</t>
-        </is>
-      </c>
+      <c r="AM3" s="5" t="n"/>
       <c r="AN3" s="5" t="n"/>
       <c r="AO3" s="5" t="n"/>
       <c r="AP3" s="5" t="n"/>
@@ -767,6 +772,9 @@
       <c r="AZ3" s="5" t="n"/>
       <c r="BA3" s="5" t="n"/>
       <c r="BB3" s="5" t="n"/>
+      <c r="BC3" s="5" t="n"/>
+      <c r="BD3" s="5" t="n"/>
+      <c r="BE3" s="5" t="n"/>
     </row>
     <row r="4">
       <c r="A4" s="7" t="inlineStr">
@@ -897,10 +905,10 @@
         <v>1</v>
       </c>
       <c r="AR4" s="7" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="AS4" s="7" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="AT4" s="7" t="n">
         <v>1</v>
@@ -918,16 +926,25 @@
         <v>1</v>
       </c>
       <c r="AY4" s="7" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="AZ4" s="7" t="n">
         <v>8</v>
       </c>
       <c r="BA4" s="7" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="BB4" s="7" t="n">
-        <v>5</v>
+        <v>8</v>
+      </c>
+      <c r="BC4" s="7" t="n">
+        <v>8</v>
+      </c>
+      <c r="BD4" s="7" t="n">
+        <v>15</v>
+      </c>
+      <c r="BE4" s="7" t="n">
+        <v>15</v>
       </c>
     </row>
     <row r="5">
@@ -997,6 +1014,9 @@
       <c r="AZ5" s="9" t="n"/>
       <c r="BA5" s="9" t="n"/>
       <c r="BB5" s="9" t="n"/>
+      <c r="BC5" s="9" t="n"/>
+      <c r="BD5" s="9" t="n"/>
+      <c r="BE5" s="9" t="n"/>
     </row>
     <row r="6">
       <c r="A6" s="5" t="inlineStr">
@@ -1211,62 +1231,77 @@
       </c>
       <c r="AQ6" s="5" t="inlineStr">
         <is>
+          <t>Q11</t>
+        </is>
+      </c>
+      <c r="AR6" s="5" t="inlineStr">
+        <is>
+          <t>Q13A</t>
+        </is>
+      </c>
+      <c r="AS6" s="5" t="inlineStr">
+        <is>
+          <t>Q13B</t>
+        </is>
+      </c>
+      <c r="AT6" s="5" t="inlineStr">
+        <is>
           <t>Q5</t>
         </is>
       </c>
-      <c r="AR6" s="5" t="inlineStr">
+      <c r="AU6" s="5" t="inlineStr">
         <is>
           <t>Q6</t>
         </is>
       </c>
-      <c r="AS6" s="5" t="inlineStr">
+      <c r="AV6" s="5" t="inlineStr">
         <is>
           <t>Q7</t>
         </is>
       </c>
-      <c r="AT6" s="5" t="inlineStr">
+      <c r="AW6" s="5" t="inlineStr">
         <is>
           <t>Q8</t>
         </is>
       </c>
-      <c r="AU6" s="5" t="inlineStr">
+      <c r="AX6" s="5" t="inlineStr">
         <is>
           <t>Q9</t>
         </is>
       </c>
-      <c r="AV6" s="5" t="inlineStr">
+      <c r="AY6" s="5" t="inlineStr">
         <is>
           <t>Q10</t>
         </is>
       </c>
-      <c r="AW6" s="5" t="inlineStr">
-        <is>
-          <t>Q11</t>
-        </is>
-      </c>
-      <c r="AX6" s="5" t="inlineStr">
-        <is>
-          <t>Q12</t>
-        </is>
-      </c>
-      <c r="AY6" s="5" t="inlineStr">
-        <is>
-          <t>Q13A</t>
-        </is>
-      </c>
       <c r="AZ6" s="5" t="inlineStr">
         <is>
-          <t>Q13B</t>
+          <t>Q12A</t>
         </is>
       </c>
       <c r="BA6" s="5" t="inlineStr">
         <is>
-          <t>Q14</t>
+          <t>Q12B</t>
         </is>
       </c>
       <c r="BB6" s="5" t="inlineStr">
         <is>
+          <t>Q14A</t>
+        </is>
+      </c>
+      <c r="BC6" s="5" t="inlineStr">
+        <is>
+          <t>Q14B</t>
+        </is>
+      </c>
+      <c r="BD6" s="5" t="inlineStr">
+        <is>
           <t>Q15</t>
+        </is>
+      </c>
+      <c r="BE6" s="5" t="inlineStr">
+        <is>
+          <t>Q16</t>
         </is>
       </c>
     </row>
@@ -1325,6 +1360,9 @@
       <c r="AZ7" s="11" t="n"/>
       <c r="BA7" s="11" t="n"/>
       <c r="BB7" s="11" t="n"/>
+      <c r="BC7" s="11" t="n"/>
+      <c r="BD7" s="11" t="n"/>
+      <c r="BE7" s="11" t="n"/>
     </row>
     <row r="8">
       <c r="A8" s="11" t="n"/>
@@ -1381,6 +1419,9 @@
       <c r="AZ8" s="11" t="n"/>
       <c r="BA8" s="11" t="n"/>
       <c r="BB8" s="11" t="n"/>
+      <c r="BC8" s="11" t="n"/>
+      <c r="BD8" s="11" t="n"/>
+      <c r="BE8" s="11" t="n"/>
     </row>
     <row r="9">
       <c r="A9" s="11" t="n"/>
@@ -1437,6 +1478,9 @@
       <c r="AZ9" s="11" t="n"/>
       <c r="BA9" s="11" t="n"/>
       <c r="BB9" s="11" t="n"/>
+      <c r="BC9" s="11" t="n"/>
+      <c r="BD9" s="11" t="n"/>
+      <c r="BE9" s="11" t="n"/>
     </row>
     <row r="10">
       <c r="A10" s="11" t="n"/>
@@ -1493,6 +1537,9 @@
       <c r="AZ10" s="11" t="n"/>
       <c r="BA10" s="11" t="n"/>
       <c r="BB10" s="11" t="n"/>
+      <c r="BC10" s="11" t="n"/>
+      <c r="BD10" s="11" t="n"/>
+      <c r="BE10" s="11" t="n"/>
     </row>
     <row r="11">
       <c r="A11" s="11" t="n"/>
@@ -1549,6 +1596,9 @@
       <c r="AZ11" s="11" t="n"/>
       <c r="BA11" s="11" t="n"/>
       <c r="BB11" s="11" t="n"/>
+      <c r="BC11" s="11" t="n"/>
+      <c r="BD11" s="11" t="n"/>
+      <c r="BE11" s="11" t="n"/>
     </row>
     <row r="12">
       <c r="A12" s="11" t="n"/>
@@ -1605,6 +1655,9 @@
       <c r="AZ12" s="11" t="n"/>
       <c r="BA12" s="11" t="n"/>
       <c r="BB12" s="11" t="n"/>
+      <c r="BC12" s="11" t="n"/>
+      <c r="BD12" s="11" t="n"/>
+      <c r="BE12" s="11" t="n"/>
     </row>
     <row r="13">
       <c r="A13" s="11" t="n"/>
@@ -1661,6 +1714,9 @@
       <c r="AZ13" s="11" t="n"/>
       <c r="BA13" s="11" t="n"/>
       <c r="BB13" s="11" t="n"/>
+      <c r="BC13" s="11" t="n"/>
+      <c r="BD13" s="11" t="n"/>
+      <c r="BE13" s="11" t="n"/>
     </row>
     <row r="14">
       <c r="A14" s="11" t="n"/>
@@ -1717,6 +1773,9 @@
       <c r="AZ14" s="11" t="n"/>
       <c r="BA14" s="11" t="n"/>
       <c r="BB14" s="11" t="n"/>
+      <c r="BC14" s="11" t="n"/>
+      <c r="BD14" s="11" t="n"/>
+      <c r="BE14" s="11" t="n"/>
     </row>
     <row r="15">
       <c r="A15" s="11" t="n"/>
@@ -1773,6 +1832,9 @@
       <c r="AZ15" s="11" t="n"/>
       <c r="BA15" s="11" t="n"/>
       <c r="BB15" s="11" t="n"/>
+      <c r="BC15" s="11" t="n"/>
+      <c r="BD15" s="11" t="n"/>
+      <c r="BE15" s="11" t="n"/>
     </row>
     <row r="16">
       <c r="A16" s="11" t="n"/>
@@ -1829,6 +1891,9 @@
       <c r="AZ16" s="11" t="n"/>
       <c r="BA16" s="11" t="n"/>
       <c r="BB16" s="11" t="n"/>
+      <c r="BC16" s="11" t="n"/>
+      <c r="BD16" s="11" t="n"/>
+      <c r="BE16" s="11" t="n"/>
     </row>
     <row r="17">
       <c r="A17" s="11" t="n"/>
@@ -1885,6 +1950,9 @@
       <c r="AZ17" s="11" t="n"/>
       <c r="BA17" s="11" t="n"/>
       <c r="BB17" s="11" t="n"/>
+      <c r="BC17" s="11" t="n"/>
+      <c r="BD17" s="11" t="n"/>
+      <c r="BE17" s="11" t="n"/>
     </row>
     <row r="18">
       <c r="A18" s="11" t="n"/>
@@ -1941,6 +2009,9 @@
       <c r="AZ18" s="11" t="n"/>
       <c r="BA18" s="11" t="n"/>
       <c r="BB18" s="11" t="n"/>
+      <c r="BC18" s="11" t="n"/>
+      <c r="BD18" s="11" t="n"/>
+      <c r="BE18" s="11" t="n"/>
     </row>
     <row r="19">
       <c r="A19" s="11" t="n"/>
@@ -1997,6 +2068,9 @@
       <c r="AZ19" s="11" t="n"/>
       <c r="BA19" s="11" t="n"/>
       <c r="BB19" s="11" t="n"/>
+      <c r="BC19" s="11" t="n"/>
+      <c r="BD19" s="11" t="n"/>
+      <c r="BE19" s="11" t="n"/>
     </row>
     <row r="20">
       <c r="A20" s="11" t="n"/>
@@ -2053,6 +2127,9 @@
       <c r="AZ20" s="11" t="n"/>
       <c r="BA20" s="11" t="n"/>
       <c r="BB20" s="11" t="n"/>
+      <c r="BC20" s="11" t="n"/>
+      <c r="BD20" s="11" t="n"/>
+      <c r="BE20" s="11" t="n"/>
     </row>
     <row r="21">
       <c r="A21" s="11" t="n"/>
@@ -2109,6 +2186,9 @@
       <c r="AZ21" s="11" t="n"/>
       <c r="BA21" s="11" t="n"/>
       <c r="BB21" s="11" t="n"/>
+      <c r="BC21" s="11" t="n"/>
+      <c r="BD21" s="11" t="n"/>
+      <c r="BE21" s="11" t="n"/>
     </row>
     <row r="22">
       <c r="A22" s="11" t="n"/>
@@ -2165,6 +2245,9 @@
       <c r="AZ22" s="11" t="n"/>
       <c r="BA22" s="11" t="n"/>
       <c r="BB22" s="11" t="n"/>
+      <c r="BC22" s="11" t="n"/>
+      <c r="BD22" s="11" t="n"/>
+      <c r="BE22" s="11" t="n"/>
     </row>
     <row r="23">
       <c r="A23" s="11" t="n"/>
@@ -2221,6 +2304,9 @@
       <c r="AZ23" s="11" t="n"/>
       <c r="BA23" s="11" t="n"/>
       <c r="BB23" s="11" t="n"/>
+      <c r="BC23" s="11" t="n"/>
+      <c r="BD23" s="11" t="n"/>
+      <c r="BE23" s="11" t="n"/>
     </row>
     <row r="24">
       <c r="A24" s="11" t="n"/>
@@ -2277,6 +2363,9 @@
       <c r="AZ24" s="11" t="n"/>
       <c r="BA24" s="11" t="n"/>
       <c r="BB24" s="11" t="n"/>
+      <c r="BC24" s="11" t="n"/>
+      <c r="BD24" s="11" t="n"/>
+      <c r="BE24" s="11" t="n"/>
     </row>
     <row r="25">
       <c r="A25" s="11" t="n"/>
@@ -2333,6 +2422,9 @@
       <c r="AZ25" s="11" t="n"/>
       <c r="BA25" s="11" t="n"/>
       <c r="BB25" s="11" t="n"/>
+      <c r="BC25" s="11" t="n"/>
+      <c r="BD25" s="11" t="n"/>
+      <c r="BE25" s="11" t="n"/>
     </row>
     <row r="26">
       <c r="A26" s="11" t="n"/>
@@ -2389,6 +2481,9 @@
       <c r="AZ26" s="11" t="n"/>
       <c r="BA26" s="11" t="n"/>
       <c r="BB26" s="11" t="n"/>
+      <c r="BC26" s="11" t="n"/>
+      <c r="BD26" s="11" t="n"/>
+      <c r="BE26" s="11" t="n"/>
     </row>
     <row r="27">
       <c r="A27" s="11" t="n"/>
@@ -2445,6 +2540,9 @@
       <c r="AZ27" s="11" t="n"/>
       <c r="BA27" s="11" t="n"/>
       <c r="BB27" s="11" t="n"/>
+      <c r="BC27" s="11" t="n"/>
+      <c r="BD27" s="11" t="n"/>
+      <c r="BE27" s="11" t="n"/>
     </row>
     <row r="28">
       <c r="A28" s="11" t="n"/>
@@ -2501,6 +2599,9 @@
       <c r="AZ28" s="11" t="n"/>
       <c r="BA28" s="11" t="n"/>
       <c r="BB28" s="11" t="n"/>
+      <c r="BC28" s="11" t="n"/>
+      <c r="BD28" s="11" t="n"/>
+      <c r="BE28" s="11" t="n"/>
     </row>
     <row r="29">
       <c r="A29" s="11" t="n"/>
@@ -2557,6 +2658,9 @@
       <c r="AZ29" s="11" t="n"/>
       <c r="BA29" s="11" t="n"/>
       <c r="BB29" s="11" t="n"/>
+      <c r="BC29" s="11" t="n"/>
+      <c r="BD29" s="11" t="n"/>
+      <c r="BE29" s="11" t="n"/>
     </row>
     <row r="30">
       <c r="A30" s="11" t="n"/>
@@ -2613,6 +2717,9 @@
       <c r="AZ30" s="11" t="n"/>
       <c r="BA30" s="11" t="n"/>
       <c r="BB30" s="11" t="n"/>
+      <c r="BC30" s="11" t="n"/>
+      <c r="BD30" s="11" t="n"/>
+      <c r="BE30" s="11" t="n"/>
     </row>
     <row r="31">
       <c r="A31" s="11" t="n"/>
@@ -2669,6 +2776,9 @@
       <c r="AZ31" s="11" t="n"/>
       <c r="BA31" s="11" t="n"/>
       <c r="BB31" s="11" t="n"/>
+      <c r="BC31" s="11" t="n"/>
+      <c r="BD31" s="11" t="n"/>
+      <c r="BE31" s="11" t="n"/>
     </row>
     <row r="32">
       <c r="A32" s="11" t="n"/>
@@ -2725,6 +2835,9 @@
       <c r="AZ32" s="11" t="n"/>
       <c r="BA32" s="11" t="n"/>
       <c r="BB32" s="11" t="n"/>
+      <c r="BC32" s="11" t="n"/>
+      <c r="BD32" s="11" t="n"/>
+      <c r="BE32" s="11" t="n"/>
     </row>
     <row r="33">
       <c r="A33" s="11" t="n"/>
@@ -2781,6 +2894,9 @@
       <c r="AZ33" s="11" t="n"/>
       <c r="BA33" s="11" t="n"/>
       <c r="BB33" s="11" t="n"/>
+      <c r="BC33" s="11" t="n"/>
+      <c r="BD33" s="11" t="n"/>
+      <c r="BE33" s="11" t="n"/>
     </row>
     <row r="34">
       <c r="A34" s="11" t="n"/>
@@ -2837,6 +2953,9 @@
       <c r="AZ34" s="11" t="n"/>
       <c r="BA34" s="11" t="n"/>
       <c r="BB34" s="11" t="n"/>
+      <c r="BC34" s="11" t="n"/>
+      <c r="BD34" s="11" t="n"/>
+      <c r="BE34" s="11" t="n"/>
     </row>
     <row r="35">
       <c r="A35" s="11" t="n"/>
@@ -2893,6 +3012,9 @@
       <c r="AZ35" s="11" t="n"/>
       <c r="BA35" s="11" t="n"/>
       <c r="BB35" s="11" t="n"/>
+      <c r="BC35" s="11" t="n"/>
+      <c r="BD35" s="11" t="n"/>
+      <c r="BE35" s="11" t="n"/>
     </row>
     <row r="36">
       <c r="A36" s="11" t="n"/>
@@ -2949,6 +3071,9 @@
       <c r="AZ36" s="11" t="n"/>
       <c r="BA36" s="11" t="n"/>
       <c r="BB36" s="11" t="n"/>
+      <c r="BC36" s="11" t="n"/>
+      <c r="BD36" s="11" t="n"/>
+      <c r="BE36" s="11" t="n"/>
     </row>
     <row r="37">
       <c r="A37" s="11" t="n"/>
@@ -3005,6 +3130,9 @@
       <c r="AZ37" s="11" t="n"/>
       <c r="BA37" s="11" t="n"/>
       <c r="BB37" s="11" t="n"/>
+      <c r="BC37" s="11" t="n"/>
+      <c r="BD37" s="11" t="n"/>
+      <c r="BE37" s="11" t="n"/>
     </row>
     <row r="38">
       <c r="A38" s="11" t="n"/>
@@ -3061,6 +3189,9 @@
       <c r="AZ38" s="11" t="n"/>
       <c r="BA38" s="11" t="n"/>
       <c r="BB38" s="11" t="n"/>
+      <c r="BC38" s="11" t="n"/>
+      <c r="BD38" s="11" t="n"/>
+      <c r="BE38" s="11" t="n"/>
     </row>
     <row r="39">
       <c r="A39" s="11" t="n"/>
@@ -3117,6 +3248,9 @@
       <c r="AZ39" s="11" t="n"/>
       <c r="BA39" s="11" t="n"/>
       <c r="BB39" s="11" t="n"/>
+      <c r="BC39" s="11" t="n"/>
+      <c r="BD39" s="11" t="n"/>
+      <c r="BE39" s="11" t="n"/>
     </row>
     <row r="40">
       <c r="A40" s="11" t="n"/>
@@ -3173,6 +3307,9 @@
       <c r="AZ40" s="11" t="n"/>
       <c r="BA40" s="11" t="n"/>
       <c r="BB40" s="11" t="n"/>
+      <c r="BC40" s="11" t="n"/>
+      <c r="BD40" s="11" t="n"/>
+      <c r="BE40" s="11" t="n"/>
     </row>
     <row r="41">
       <c r="A41" s="11" t="n"/>
@@ -3229,6 +3366,9 @@
       <c r="AZ41" s="11" t="n"/>
       <c r="BA41" s="11" t="n"/>
       <c r="BB41" s="11" t="n"/>
+      <c r="BC41" s="11" t="n"/>
+      <c r="BD41" s="11" t="n"/>
+      <c r="BE41" s="11" t="n"/>
     </row>
     <row r="42">
       <c r="A42" s="11" t="n"/>
@@ -3285,6 +3425,9 @@
       <c r="AZ42" s="11" t="n"/>
       <c r="BA42" s="11" t="n"/>
       <c r="BB42" s="11" t="n"/>
+      <c r="BC42" s="11" t="n"/>
+      <c r="BD42" s="11" t="n"/>
+      <c r="BE42" s="11" t="n"/>
     </row>
     <row r="43">
       <c r="A43" s="11" t="n"/>
@@ -3341,6 +3484,9 @@
       <c r="AZ43" s="11" t="n"/>
       <c r="BA43" s="11" t="n"/>
       <c r="BB43" s="11" t="n"/>
+      <c r="BC43" s="11" t="n"/>
+      <c r="BD43" s="11" t="n"/>
+      <c r="BE43" s="11" t="n"/>
     </row>
     <row r="44">
       <c r="A44" s="11" t="n"/>
@@ -3397,6 +3543,9 @@
       <c r="AZ44" s="11" t="n"/>
       <c r="BA44" s="11" t="n"/>
       <c r="BB44" s="11" t="n"/>
+      <c r="BC44" s="11" t="n"/>
+      <c r="BD44" s="11" t="n"/>
+      <c r="BE44" s="11" t="n"/>
     </row>
     <row r="45">
       <c r="A45" s="11" t="n"/>
@@ -3453,6 +3602,9 @@
       <c r="AZ45" s="11" t="n"/>
       <c r="BA45" s="11" t="n"/>
       <c r="BB45" s="11" t="n"/>
+      <c r="BC45" s="11" t="n"/>
+      <c r="BD45" s="11" t="n"/>
+      <c r="BE45" s="11" t="n"/>
     </row>
     <row r="46">
       <c r="A46" s="11" t="n"/>
@@ -3509,6 +3661,9 @@
       <c r="AZ46" s="11" t="n"/>
       <c r="BA46" s="11" t="n"/>
       <c r="BB46" s="11" t="n"/>
+      <c r="BC46" s="11" t="n"/>
+      <c r="BD46" s="11" t="n"/>
+      <c r="BE46" s="11" t="n"/>
     </row>
     <row r="47">
       <c r="A47" s="11" t="n"/>
@@ -3565,6 +3720,9 @@
       <c r="AZ47" s="11" t="n"/>
       <c r="BA47" s="11" t="n"/>
       <c r="BB47" s="11" t="n"/>
+      <c r="BC47" s="11" t="n"/>
+      <c r="BD47" s="11" t="n"/>
+      <c r="BE47" s="11" t="n"/>
     </row>
     <row r="48">
       <c r="A48" s="11" t="n"/>
@@ -3621,6 +3779,9 @@
       <c r="AZ48" s="11" t="n"/>
       <c r="BA48" s="11" t="n"/>
       <c r="BB48" s="11" t="n"/>
+      <c r="BC48" s="11" t="n"/>
+      <c r="BD48" s="11" t="n"/>
+      <c r="BE48" s="11" t="n"/>
     </row>
     <row r="49">
       <c r="A49" s="11" t="n"/>
@@ -3677,6 +3838,9 @@
       <c r="AZ49" s="11" t="n"/>
       <c r="BA49" s="11" t="n"/>
       <c r="BB49" s="11" t="n"/>
+      <c r="BC49" s="11" t="n"/>
+      <c r="BD49" s="11" t="n"/>
+      <c r="BE49" s="11" t="n"/>
     </row>
     <row r="50">
       <c r="A50" s="11" t="n"/>
@@ -3733,6 +3897,9 @@
       <c r="AZ50" s="11" t="n"/>
       <c r="BA50" s="11" t="n"/>
       <c r="BB50" s="11" t="n"/>
+      <c r="BC50" s="11" t="n"/>
+      <c r="BD50" s="11" t="n"/>
+      <c r="BE50" s="11" t="n"/>
     </row>
     <row r="51">
       <c r="A51" s="11" t="n"/>
@@ -3789,6 +3956,9 @@
       <c r="AZ51" s="11" t="n"/>
       <c r="BA51" s="11" t="n"/>
       <c r="BB51" s="11" t="n"/>
+      <c r="BC51" s="11" t="n"/>
+      <c r="BD51" s="11" t="n"/>
+      <c r="BE51" s="11" t="n"/>
     </row>
     <row r="52">
       <c r="A52" s="11" t="n"/>
@@ -3845,6 +4015,9 @@
       <c r="AZ52" s="11" t="n"/>
       <c r="BA52" s="11" t="n"/>
       <c r="BB52" s="11" t="n"/>
+      <c r="BC52" s="11" t="n"/>
+      <c r="BD52" s="11" t="n"/>
+      <c r="BE52" s="11" t="n"/>
     </row>
     <row r="53">
       <c r="A53" s="11" t="n"/>
@@ -3901,6 +4074,9 @@
       <c r="AZ53" s="11" t="n"/>
       <c r="BA53" s="11" t="n"/>
       <c r="BB53" s="11" t="n"/>
+      <c r="BC53" s="11" t="n"/>
+      <c r="BD53" s="11" t="n"/>
+      <c r="BE53" s="11" t="n"/>
     </row>
     <row r="54">
       <c r="A54" s="11" t="n"/>
@@ -3957,6 +4133,9 @@
       <c r="AZ54" s="11" t="n"/>
       <c r="BA54" s="11" t="n"/>
       <c r="BB54" s="11" t="n"/>
+      <c r="BC54" s="11" t="n"/>
+      <c r="BD54" s="11" t="n"/>
+      <c r="BE54" s="11" t="n"/>
     </row>
     <row r="55">
       <c r="A55" s="11" t="n"/>
@@ -4013,6 +4192,9 @@
       <c r="AZ55" s="11" t="n"/>
       <c r="BA55" s="11" t="n"/>
       <c r="BB55" s="11" t="n"/>
+      <c r="BC55" s="11" t="n"/>
+      <c r="BD55" s="11" t="n"/>
+      <c r="BE55" s="11" t="n"/>
     </row>
     <row r="56">
       <c r="A56" s="11" t="n"/>
@@ -4069,6 +4251,9 @@
       <c r="AZ56" s="11" t="n"/>
       <c r="BA56" s="11" t="n"/>
       <c r="BB56" s="11" t="n"/>
+      <c r="BC56" s="11" t="n"/>
+      <c r="BD56" s="11" t="n"/>
+      <c r="BE56" s="11" t="n"/>
     </row>
     <row r="57">
       <c r="A57" s="11" t="n"/>
@@ -4125,6 +4310,9 @@
       <c r="AZ57" s="11" t="n"/>
       <c r="BA57" s="11" t="n"/>
       <c r="BB57" s="11" t="n"/>
+      <c r="BC57" s="11" t="n"/>
+      <c r="BD57" s="11" t="n"/>
+      <c r="BE57" s="11" t="n"/>
     </row>
     <row r="58">
       <c r="A58" s="11" t="n"/>
@@ -4181,6 +4369,9 @@
       <c r="AZ58" s="11" t="n"/>
       <c r="BA58" s="11" t="n"/>
       <c r="BB58" s="11" t="n"/>
+      <c r="BC58" s="11" t="n"/>
+      <c r="BD58" s="11" t="n"/>
+      <c r="BE58" s="11" t="n"/>
     </row>
     <row r="59">
       <c r="A59" s="11" t="n"/>
@@ -4237,6 +4428,9 @@
       <c r="AZ59" s="11" t="n"/>
       <c r="BA59" s="11" t="n"/>
       <c r="BB59" s="11" t="n"/>
+      <c r="BC59" s="11" t="n"/>
+      <c r="BD59" s="11" t="n"/>
+      <c r="BE59" s="11" t="n"/>
     </row>
     <row r="60">
       <c r="A60" s="11" t="n"/>
@@ -4293,6 +4487,9 @@
       <c r="AZ60" s="11" t="n"/>
       <c r="BA60" s="11" t="n"/>
       <c r="BB60" s="11" t="n"/>
+      <c r="BC60" s="11" t="n"/>
+      <c r="BD60" s="11" t="n"/>
+      <c r="BE60" s="11" t="n"/>
     </row>
     <row r="61">
       <c r="A61" s="11" t="n"/>
@@ -4349,6 +4546,9 @@
       <c r="AZ61" s="11" t="n"/>
       <c r="BA61" s="11" t="n"/>
       <c r="BB61" s="11" t="n"/>
+      <c r="BC61" s="11" t="n"/>
+      <c r="BD61" s="11" t="n"/>
+      <c r="BE61" s="11" t="n"/>
     </row>
     <row r="62">
       <c r="A62" s="11" t="n"/>
@@ -4405,6 +4605,9 @@
       <c r="AZ62" s="11" t="n"/>
       <c r="BA62" s="11" t="n"/>
       <c r="BB62" s="11" t="n"/>
+      <c r="BC62" s="11" t="n"/>
+      <c r="BD62" s="11" t="n"/>
+      <c r="BE62" s="11" t="n"/>
     </row>
     <row r="63">
       <c r="A63" s="11" t="n"/>
@@ -4461,6 +4664,9 @@
       <c r="AZ63" s="11" t="n"/>
       <c r="BA63" s="11" t="n"/>
       <c r="BB63" s="11" t="n"/>
+      <c r="BC63" s="11" t="n"/>
+      <c r="BD63" s="11" t="n"/>
+      <c r="BE63" s="11" t="n"/>
     </row>
     <row r="64">
       <c r="A64" s="11" t="n"/>
@@ -4517,6 +4723,9 @@
       <c r="AZ64" s="11" t="n"/>
       <c r="BA64" s="11" t="n"/>
       <c r="BB64" s="11" t="n"/>
+      <c r="BC64" s="11" t="n"/>
+      <c r="BD64" s="11" t="n"/>
+      <c r="BE64" s="11" t="n"/>
     </row>
     <row r="65">
       <c r="A65" s="11" t="n"/>
@@ -4573,6 +4782,9 @@
       <c r="AZ65" s="11" t="n"/>
       <c r="BA65" s="11" t="n"/>
       <c r="BB65" s="11" t="n"/>
+      <c r="BC65" s="11" t="n"/>
+      <c r="BD65" s="11" t="n"/>
+      <c r="BE65" s="11" t="n"/>
     </row>
     <row r="66">
       <c r="A66" s="11" t="n"/>
@@ -4629,6 +4841,9 @@
       <c r="AZ66" s="11" t="n"/>
       <c r="BA66" s="11" t="n"/>
       <c r="BB66" s="11" t="n"/>
+      <c r="BC66" s="11" t="n"/>
+      <c r="BD66" s="11" t="n"/>
+      <c r="BE66" s="11" t="n"/>
     </row>
     <row r="67">
       <c r="A67" s="5" t="inlineStr">
@@ -4842,6 +5057,18 @@
         <f>COUNTA(BB7:BB66)</f>
         <v/>
       </c>
+      <c r="BC67" s="11">
+        <f>COUNTA(BC7:BC66)</f>
+        <v/>
+      </c>
+      <c r="BD67" s="11">
+        <f>COUNTA(BD7:BD66)</f>
+        <v/>
+      </c>
+      <c r="BE67" s="11">
+        <f>COUNTA(BE7:BE66)</f>
+        <v/>
+      </c>
     </row>
     <row r="68">
       <c r="A68" s="7" t="inlineStr">
@@ -5055,6 +5282,18 @@
         <f>COUNTIF(BB7:BB66,"&gt;="&amp;0.65*BB4)</f>
         <v/>
       </c>
+      <c r="BC68" s="13">
+        <f>COUNTIF(BC7:BC66,"&gt;="&amp;0.65*BC4)</f>
+        <v/>
+      </c>
+      <c r="BD68" s="13">
+        <f>COUNTIF(BD7:BD66,"&gt;="&amp;0.65*BD4)</f>
+        <v/>
+      </c>
+      <c r="BE68" s="13">
+        <f>COUNTIF(BE7:BE66,"&gt;="&amp;0.65*BE4)</f>
+        <v/>
+      </c>
     </row>
     <row r="69">
       <c r="A69" s="5" t="inlineStr">
@@ -5065,207 +5304,219 @@
       <c r="B69" s="5" t="n"/>
       <c r="C69" s="6" t="n"/>
       <c r="D69" s="11">
-        <f>IF(D67&gt;0,D68/D67*100,"-")</f>
+        <f>IF(D67&gt;0,ROUND(D68/D67*100,2),"-")</f>
         <v/>
       </c>
       <c r="E69" s="11">
-        <f>IF(E67&gt;0,E68/E67*100,"-")</f>
+        <f>IF(E67&gt;0,ROUND(E68/E67*100,2),"-")</f>
         <v/>
       </c>
       <c r="F69" s="11">
-        <f>IF(F67&gt;0,F68/F67*100,"-")</f>
+        <f>IF(F67&gt;0,ROUND(F68/F67*100,2),"-")</f>
         <v/>
       </c>
       <c r="G69" s="11">
-        <f>IF(G67&gt;0,G68/G67*100,"-")</f>
+        <f>IF(G67&gt;0,ROUND(G68/G67*100,2),"-")</f>
         <v/>
       </c>
       <c r="H69" s="11">
-        <f>IF(H67&gt;0,H68/H67*100,"-")</f>
+        <f>IF(H67&gt;0,ROUND(H68/H67*100,2),"-")</f>
         <v/>
       </c>
       <c r="I69" s="11">
-        <f>IF(I67&gt;0,I68/I67*100,"-")</f>
+        <f>IF(I67&gt;0,ROUND(I68/I67*100,2),"-")</f>
         <v/>
       </c>
       <c r="J69" s="11">
-        <f>IF(J67&gt;0,J68/J67*100,"-")</f>
+        <f>IF(J67&gt;0,ROUND(J68/J67*100,2),"-")</f>
         <v/>
       </c>
       <c r="K69" s="11">
-        <f>IF(K67&gt;0,K68/K67*100,"-")</f>
+        <f>IF(K67&gt;0,ROUND(K68/K67*100,2),"-")</f>
         <v/>
       </c>
       <c r="L69" s="11">
-        <f>IF(L67&gt;0,L68/L67*100,"-")</f>
+        <f>IF(L67&gt;0,ROUND(L68/L67*100,2),"-")</f>
         <v/>
       </c>
       <c r="M69" s="11">
-        <f>IF(M67&gt;0,M68/M67*100,"-")</f>
+        <f>IF(M67&gt;0,ROUND(M68/M67*100,2),"-")</f>
         <v/>
       </c>
       <c r="N69" s="11">
-        <f>IF(N67&gt;0,N68/N67*100,"-")</f>
+        <f>IF(N67&gt;0,ROUND(N68/N67*100,2),"-")</f>
         <v/>
       </c>
       <c r="O69" s="11">
-        <f>IF(O67&gt;0,O68/O67*100,"-")</f>
+        <f>IF(O67&gt;0,ROUND(O68/O67*100,2),"-")</f>
         <v/>
       </c>
       <c r="P69" s="11">
-        <f>IF(P67&gt;0,P68/P67*100,"-")</f>
+        <f>IF(P67&gt;0,ROUND(P68/P67*100,2),"-")</f>
         <v/>
       </c>
       <c r="Q69" s="11">
-        <f>IF(Q67&gt;0,Q68/Q67*100,"-")</f>
+        <f>IF(Q67&gt;0,ROUND(Q68/Q67*100,2),"-")</f>
         <v/>
       </c>
       <c r="R69" s="11">
-        <f>IF(R67&gt;0,R68/R67*100,"-")</f>
+        <f>IF(R67&gt;0,ROUND(R68/R67*100,2),"-")</f>
         <v/>
       </c>
       <c r="S69" s="11">
-        <f>IF(S67&gt;0,S68/S67*100,"-")</f>
+        <f>IF(S67&gt;0,ROUND(S68/S67*100,2),"-")</f>
         <v/>
       </c>
       <c r="T69" s="11">
-        <f>IF(T67&gt;0,T68/T67*100,"-")</f>
+        <f>IF(T67&gt;0,ROUND(T68/T67*100,2),"-")</f>
         <v/>
       </c>
       <c r="U69" s="11">
-        <f>IF(U67&gt;0,U68/U67*100,"-")</f>
+        <f>IF(U67&gt;0,ROUND(U68/U67*100,2),"-")</f>
         <v/>
       </c>
       <c r="V69" s="11">
-        <f>IF(V67&gt;0,V68/V67*100,"-")</f>
+        <f>IF(V67&gt;0,ROUND(V68/V67*100,2),"-")</f>
         <v/>
       </c>
       <c r="W69" s="11">
-        <f>IF(W67&gt;0,W68/W67*100,"-")</f>
+        <f>IF(W67&gt;0,ROUND(W68/W67*100,2),"-")</f>
         <v/>
       </c>
       <c r="X69" s="11">
-        <f>IF(X67&gt;0,X68/X67*100,"-")</f>
+        <f>IF(X67&gt;0,ROUND(X68/X67*100,2),"-")</f>
         <v/>
       </c>
       <c r="Y69" s="11">
-        <f>IF(Y67&gt;0,Y68/Y67*100,"-")</f>
+        <f>IF(Y67&gt;0,ROUND(Y68/Y67*100,2),"-")</f>
         <v/>
       </c>
       <c r="Z69" s="11">
-        <f>IF(Z67&gt;0,Z68/Z67*100,"-")</f>
+        <f>IF(Z67&gt;0,ROUND(Z68/Z67*100,2),"-")</f>
         <v/>
       </c>
       <c r="AA69" s="11">
-        <f>IF(AA67&gt;0,AA68/AA67*100,"-")</f>
+        <f>IF(AA67&gt;0,ROUND(AA68/AA67*100,2),"-")</f>
         <v/>
       </c>
       <c r="AB69" s="11">
-        <f>IF(AB67&gt;0,AB68/AB67*100,"-")</f>
+        <f>IF(AB67&gt;0,ROUND(AB68/AB67*100,2),"-")</f>
         <v/>
       </c>
       <c r="AC69" s="11">
-        <f>IF(AC67&gt;0,AC68/AC67*100,"-")</f>
+        <f>IF(AC67&gt;0,ROUND(AC68/AC67*100,2),"-")</f>
         <v/>
       </c>
       <c r="AD69" s="11">
-        <f>IF(AD67&gt;0,AD68/AD67*100,"-")</f>
+        <f>IF(AD67&gt;0,ROUND(AD68/AD67*100,2),"-")</f>
         <v/>
       </c>
       <c r="AE69" s="11">
-        <f>IF(AE67&gt;0,AE68/AE67*100,"-")</f>
+        <f>IF(AE67&gt;0,ROUND(AE68/AE67*100,2),"-")</f>
         <v/>
       </c>
       <c r="AF69" s="11">
-        <f>IF(AF67&gt;0,AF68/AF67*100,"-")</f>
+        <f>IF(AF67&gt;0,ROUND(AF68/AF67*100,2),"-")</f>
         <v/>
       </c>
       <c r="AG69" s="11">
-        <f>IF(AG67&gt;0,AG68/AG67*100,"-")</f>
+        <f>IF(AG67&gt;0,ROUND(AG68/AG67*100,2),"-")</f>
         <v/>
       </c>
       <c r="AH69" s="11">
-        <f>IF(AH67&gt;0,AH68/AH67*100,"-")</f>
+        <f>IF(AH67&gt;0,ROUND(AH68/AH67*100,2),"-")</f>
         <v/>
       </c>
       <c r="AI69" s="11">
-        <f>IF(AI67&gt;0,AI68/AI67*100,"-")</f>
+        <f>IF(AI67&gt;0,ROUND(AI68/AI67*100,2),"-")</f>
         <v/>
       </c>
       <c r="AJ69" s="11">
-        <f>IF(AJ67&gt;0,AJ68/AJ67*100,"-")</f>
+        <f>IF(AJ67&gt;0,ROUND(AJ68/AJ67*100,2),"-")</f>
         <v/>
       </c>
       <c r="AK69" s="11">
-        <f>IF(AK67&gt;0,AK68/AK67*100,"-")</f>
+        <f>IF(AK67&gt;0,ROUND(AK68/AK67*100,2),"-")</f>
         <v/>
       </c>
       <c r="AL69" s="11">
-        <f>IF(AL67&gt;0,AL68/AL67*100,"-")</f>
+        <f>IF(AL67&gt;0,ROUND(AL68/AL67*100,2),"-")</f>
         <v/>
       </c>
       <c r="AM69" s="11">
-        <f>IF(AM67&gt;0,AM68/AM67*100,"-")</f>
+        <f>IF(AM67&gt;0,ROUND(AM68/AM67*100,2),"-")</f>
         <v/>
       </c>
       <c r="AN69" s="11">
-        <f>IF(AN67&gt;0,AN68/AN67*100,"-")</f>
+        <f>IF(AN67&gt;0,ROUND(AN68/AN67*100,2),"-")</f>
         <v/>
       </c>
       <c r="AO69" s="11">
-        <f>IF(AO67&gt;0,AO68/AO67*100,"-")</f>
+        <f>IF(AO67&gt;0,ROUND(AO68/AO67*100,2),"-")</f>
         <v/>
       </c>
       <c r="AP69" s="11">
-        <f>IF(AP67&gt;0,AP68/AP67*100,"-")</f>
+        <f>IF(AP67&gt;0,ROUND(AP68/AP67*100,2),"-")</f>
         <v/>
       </c>
       <c r="AQ69" s="11">
-        <f>IF(AQ67&gt;0,AQ68/AQ67*100,"-")</f>
+        <f>IF(AQ67&gt;0,ROUND(AQ68/AQ67*100,2),"-")</f>
         <v/>
       </c>
       <c r="AR69" s="11">
-        <f>IF(AR67&gt;0,AR68/AR67*100,"-")</f>
+        <f>IF(AR67&gt;0,ROUND(AR68/AR67*100,2),"-")</f>
         <v/>
       </c>
       <c r="AS69" s="11">
-        <f>IF(AS67&gt;0,AS68/AS67*100,"-")</f>
+        <f>IF(AS67&gt;0,ROUND(AS68/AS67*100,2),"-")</f>
         <v/>
       </c>
       <c r="AT69" s="11">
-        <f>IF(AT67&gt;0,AT68/AT67*100,"-")</f>
+        <f>IF(AT67&gt;0,ROUND(AT68/AT67*100,2),"-")</f>
         <v/>
       </c>
       <c r="AU69" s="11">
-        <f>IF(AU67&gt;0,AU68/AU67*100,"-")</f>
+        <f>IF(AU67&gt;0,ROUND(AU68/AU67*100,2),"-")</f>
         <v/>
       </c>
       <c r="AV69" s="11">
-        <f>IF(AV67&gt;0,AV68/AV67*100,"-")</f>
+        <f>IF(AV67&gt;0,ROUND(AV68/AV67*100,2),"-")</f>
         <v/>
       </c>
       <c r="AW69" s="11">
-        <f>IF(AW67&gt;0,AW68/AW67*100,"-")</f>
+        <f>IF(AW67&gt;0,ROUND(AW68/AW67*100,2),"-")</f>
         <v/>
       </c>
       <c r="AX69" s="11">
-        <f>IF(AX67&gt;0,AX68/AX67*100,"-")</f>
+        <f>IF(AX67&gt;0,ROUND(AX68/AX67*100,2),"-")</f>
         <v/>
       </c>
       <c r="AY69" s="11">
-        <f>IF(AY67&gt;0,AY68/AY67*100,"-")</f>
+        <f>IF(AY67&gt;0,ROUND(AY68/AY67*100,2),"-")</f>
         <v/>
       </c>
       <c r="AZ69" s="11">
-        <f>IF(AZ67&gt;0,AZ68/AZ67*100,"-")</f>
+        <f>IF(AZ67&gt;0,ROUND(AZ68/AZ67*100,2),"-")</f>
         <v/>
       </c>
       <c r="BA69" s="11">
-        <f>IF(BA67&gt;0,BA68/BA67*100,"-")</f>
+        <f>IF(BA67&gt;0,ROUND(BA68/BA67*100,2),"-")</f>
         <v/>
       </c>
       <c r="BB69" s="11">
-        <f>IF(BB67&gt;0,BB68/BB67*100,"-")</f>
+        <f>IF(BB67&gt;0,ROUND(BB68/BB67*100,2),"-")</f>
+        <v/>
+      </c>
+      <c r="BC69" s="11">
+        <f>IF(BC67&gt;0,ROUND(BC68/BC67*100,2),"-")</f>
+        <v/>
+      </c>
+      <c r="BD69" s="11">
+        <f>IF(BD67&gt;0,ROUND(BD68/BD67*100,2),"-")</f>
+        <v/>
+      </c>
+      <c r="BE69" s="11">
+        <f>IF(BE67&gt;0,ROUND(BE68/BE67*100,2),"-")</f>
         <v/>
       </c>
     </row>
@@ -5319,7 +5570,7 @@
       <c r="AK70" s="11" t="n"/>
       <c r="AL70" s="11" t="n"/>
       <c r="AM70" s="11">
-        <f>IFERROR(ROUND(SUMPRODUCT(AM69:BB69,AM4:BB4)/SUM(AM4:BB4), 2),"-")</f>
+        <f>IFERROR(ROUND(SUMPRODUCT(AM69:BE69,AM4:BE4)/SUM(AM4:BE4), 2),"-")</f>
         <v/>
       </c>
       <c r="AN70" s="11" t="n"/>
@@ -5337,6 +5588,9 @@
       <c r="AZ70" s="11" t="n"/>
       <c r="BA70" s="11" t="n"/>
       <c r="BB70" s="11" t="n"/>
+      <c r="BC70" s="11" t="n"/>
+      <c r="BD70" s="11" t="n"/>
+      <c r="BE70" s="11" t="n"/>
     </row>
     <row r="71">
       <c r="A71" s="5" t="inlineStr">
@@ -5406,6 +5660,9 @@
       <c r="AZ71" s="11" t="n"/>
       <c r="BA71" s="11" t="n"/>
       <c r="BB71" s="11" t="n"/>
+      <c r="BC71" s="11" t="n"/>
+      <c r="BD71" s="11" t="n"/>
+      <c r="BE71" s="11" t="n"/>
     </row>
     <row r="73">
       <c r="A73" s="9" t="inlineStr">
@@ -5413,33 +5670,24 @@
           <t>CO</t>
         </is>
       </c>
-      <c r="B73" s="14" t="n"/>
-      <c r="C73" s="9" t="inlineStr">
+      <c r="B73" s="9" t="inlineStr">
         <is>
           <t>CO Wise Average Percentage of students who got more than 65% of marks</t>
         </is>
       </c>
-      <c r="D73" s="14" t="n"/>
+      <c r="C73" s="14" t="n"/>
+      <c r="D73" s="9" t="inlineStr">
+        <is>
+          <t>Overall CO Attainment Level (&gt;=85:3,&gt;=75:2,&gt;=65:1,&lt;65:0)</t>
+        </is>
+      </c>
       <c r="E73" s="14" t="n"/>
       <c r="F73" s="14" t="n"/>
       <c r="G73" s="14" t="n"/>
       <c r="H73" s="14" t="n"/>
       <c r="I73" s="14" t="n"/>
       <c r="J73" s="14" t="n"/>
-      <c r="K73" s="9" t="inlineStr">
-        <is>
-          <t>Overall CO Attainment Level (&gt;=85:3,&gt;=75:2,&gt;=65:1,&lt;65:0)</t>
-        </is>
-      </c>
-      <c r="L73" s="14" t="n"/>
-      <c r="M73" s="14" t="n"/>
-      <c r="N73" s="14" t="n"/>
-      <c r="O73" s="14" t="n"/>
-      <c r="P73" s="14" t="n"/>
-      <c r="Q73" s="14" t="n"/>
-      <c r="R73" s="14" t="n"/>
-      <c r="S73" s="14" t="n"/>
-      <c r="T73" s="14" t="n"/>
+      <c r="K73" s="14" t="n"/>
     </row>
     <row r="74">
       <c r="A74" s="11" t="inlineStr">
@@ -5447,31 +5695,22 @@
           <t>CO1</t>
         </is>
       </c>
-      <c r="B74" s="14" t="n"/>
-      <c r="C74" s="11">
-        <f>IFERROR(ROUND((SUMPRODUCT(D69:S69,D4:S4)/SUM(D4:S4)+SUMPRODUCT(AM69:BB69,AM4:BB4)/SUM(AM4:BB4))/2,2),"-")</f>
-        <v/>
-      </c>
-      <c r="D74" s="14" t="n"/>
+      <c r="B74" s="11">
+        <f>IFERROR(ROUND((SUMPRODUCT(D69:S69,D4:S4)/SUM(D4:S4))/1,2),"-")</f>
+        <v/>
+      </c>
+      <c r="C74" s="14" t="n"/>
+      <c r="D74" s="11">
+        <f>IF(B74&gt;=85,3,IF(B74&gt;=75,2,IF(B74&gt;=65,1,0)))</f>
+        <v/>
+      </c>
       <c r="E74" s="14" t="n"/>
       <c r="F74" s="14" t="n"/>
       <c r="G74" s="14" t="n"/>
       <c r="H74" s="14" t="n"/>
       <c r="I74" s="14" t="n"/>
       <c r="J74" s="14" t="n"/>
-      <c r="K74" s="11">
-        <f>IF(C74&gt;=85,3,IF(C74&gt;=75,2,IF(C74&gt;=65,1,0)))</f>
-        <v/>
-      </c>
-      <c r="L74" s="14" t="n"/>
-      <c r="M74" s="14" t="n"/>
-      <c r="N74" s="14" t="n"/>
-      <c r="O74" s="14" t="n"/>
-      <c r="P74" s="14" t="n"/>
-      <c r="Q74" s="14" t="n"/>
-      <c r="R74" s="14" t="n"/>
-      <c r="S74" s="14" t="n"/>
-      <c r="T74" s="14" t="n"/>
+      <c r="K74" s="14" t="n"/>
     </row>
     <row r="75">
       <c r="A75" s="11" t="inlineStr">
@@ -5479,31 +5718,22 @@
           <t>CO2</t>
         </is>
       </c>
-      <c r="B75" s="14" t="n"/>
-      <c r="C75" s="11">
-        <f>IFERROR(ROUND((SUMPRODUCT(T69:Z69,T4:Z4)/SUM(T4:Z4))/1,2),"-")</f>
-        <v/>
-      </c>
-      <c r="D75" s="14" t="n"/>
+      <c r="B75" s="11">
+        <f>IFERROR(ROUND((SUMPRODUCT(T69:Z69,T4:Z4)/SUM(T4:Z4)+SUMPRODUCT(AM69:AS69,AM4:AS4)/SUM(AM4:AS4))/2,2),"-")</f>
+        <v/>
+      </c>
+      <c r="C75" s="14" t="n"/>
+      <c r="D75" s="11">
+        <f>IF(B75&gt;=85,3,IF(B75&gt;=75,2,IF(B75&gt;=65,1,0)))</f>
+        <v/>
+      </c>
       <c r="E75" s="14" t="n"/>
       <c r="F75" s="14" t="n"/>
       <c r="G75" s="14" t="n"/>
       <c r="H75" s="14" t="n"/>
       <c r="I75" s="14" t="n"/>
       <c r="J75" s="14" t="n"/>
-      <c r="K75" s="11">
-        <f>IF(C75&gt;=85,3,IF(C75&gt;=75,2,IF(C75&gt;=65,1,0)))</f>
-        <v/>
-      </c>
-      <c r="L75" s="14" t="n"/>
-      <c r="M75" s="14" t="n"/>
-      <c r="N75" s="14" t="n"/>
-      <c r="O75" s="14" t="n"/>
-      <c r="P75" s="14" t="n"/>
-      <c r="Q75" s="14" t="n"/>
-      <c r="R75" s="14" t="n"/>
-      <c r="S75" s="14" t="n"/>
-      <c r="T75" s="14" t="n"/>
+      <c r="K75" s="14" t="n"/>
     </row>
     <row r="76">
       <c r="A76" s="11" t="inlineStr">
@@ -5511,75 +5741,60 @@
           <t>CO3</t>
         </is>
       </c>
-      <c r="B76" s="14" t="n"/>
-      <c r="C76" s="11">
-        <f>IFERROR(ROUND((SUMPRODUCT(AA69:AL69,AA4:AL4)/SUM(AA4:AL4))/1,2),"-")</f>
-        <v/>
-      </c>
-      <c r="D76" s="14" t="n"/>
+      <c r="B76" s="11">
+        <f>IFERROR(ROUND((SUMPRODUCT(AA69:AL69,AA4:AL4)/SUM(AA4:AL4)+SUMPRODUCT(AT69:BE69,AT4:BE4)/SUM(AT4:BE4))/2,2),"-")</f>
+        <v/>
+      </c>
+      <c r="C76" s="14" t="n"/>
+      <c r="D76" s="11">
+        <f>IF(B76&gt;=85,3,IF(B76&gt;=75,2,IF(B76&gt;=65,1,0)))</f>
+        <v/>
+      </c>
       <c r="E76" s="14" t="n"/>
       <c r="F76" s="14" t="n"/>
       <c r="G76" s="14" t="n"/>
       <c r="H76" s="14" t="n"/>
       <c r="I76" s="14" t="n"/>
       <c r="J76" s="14" t="n"/>
-      <c r="K76" s="11">
-        <f>IF(C76&gt;=85,3,IF(C76&gt;=75,2,IF(C76&gt;=65,1,0)))</f>
-        <v/>
-      </c>
-      <c r="L76" s="14" t="n"/>
-      <c r="M76" s="14" t="n"/>
-      <c r="N76" s="14" t="n"/>
-      <c r="O76" s="14" t="n"/>
-      <c r="P76" s="14" t="n"/>
-      <c r="Q76" s="14" t="n"/>
-      <c r="R76" s="14" t="n"/>
-      <c r="S76" s="14" t="n"/>
-      <c r="T76" s="14" t="n"/>
+      <c r="K76" s="14" t="n"/>
     </row>
   </sheetData>
-  <mergeCells count="41">
+  <mergeCells count="35">
     <mergeCell ref="T1:AL1"/>
-    <mergeCell ref="A73:B73"/>
     <mergeCell ref="D71:S71"/>
-    <mergeCell ref="D3:S3"/>
     <mergeCell ref="T70:AL70"/>
-    <mergeCell ref="K73:T73"/>
     <mergeCell ref="A3:C3"/>
-    <mergeCell ref="C74:J74"/>
     <mergeCell ref="A2:C2"/>
-    <mergeCell ref="AM3:BB3"/>
-    <mergeCell ref="C73:J73"/>
     <mergeCell ref="D5:S5"/>
     <mergeCell ref="A71:C71"/>
     <mergeCell ref="A5:C5"/>
-    <mergeCell ref="A75:B75"/>
-    <mergeCell ref="T3:AL3"/>
-    <mergeCell ref="K74:T74"/>
-    <mergeCell ref="A74:B74"/>
+    <mergeCell ref="D76:K76"/>
+    <mergeCell ref="AM2:AS2"/>
+    <mergeCell ref="AM1:BE1"/>
     <mergeCell ref="A4:C4"/>
-    <mergeCell ref="AM2:BB2"/>
-    <mergeCell ref="C75:J75"/>
     <mergeCell ref="D1:S1"/>
+    <mergeCell ref="D75:K75"/>
+    <mergeCell ref="B73:C73"/>
     <mergeCell ref="A68:C68"/>
     <mergeCell ref="T5:AL5"/>
     <mergeCell ref="AA2:AL2"/>
-    <mergeCell ref="A76:B76"/>
+    <mergeCell ref="AT2:BE2"/>
     <mergeCell ref="A67:C67"/>
-    <mergeCell ref="AM71:BB71"/>
-    <mergeCell ref="C76:J76"/>
-    <mergeCell ref="K76:T76"/>
+    <mergeCell ref="AM71:BE71"/>
     <mergeCell ref="D2:S2"/>
+    <mergeCell ref="B74:C74"/>
+    <mergeCell ref="D74:K74"/>
     <mergeCell ref="A1:C1"/>
-    <mergeCell ref="K75:T75"/>
     <mergeCell ref="D70:S70"/>
+    <mergeCell ref="AM5:BE5"/>
     <mergeCell ref="T71:AL71"/>
-    <mergeCell ref="AM5:BB5"/>
+    <mergeCell ref="D73:K73"/>
+    <mergeCell ref="B76:C76"/>
     <mergeCell ref="A70:C70"/>
-    <mergeCell ref="AM1:BB1"/>
     <mergeCell ref="T2:Z2"/>
     <mergeCell ref="A69:C69"/>
-    <mergeCell ref="AM70:BB70"/>
+    <mergeCell ref="AM70:BE70"/>
+    <mergeCell ref="B75:C75"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>